<commit_message>
Replace A3 simulation results and graphs
</commit_message>
<xml_diff>
--- a/A3.xlsx
+++ b/A3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17123"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -81,8 +81,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -147,6 +147,62 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Simulation 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -177,7 +233,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -798,7 +866,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6B45-41BC-832C-225F9A2781F9}"/>
             </c:ext>
@@ -828,7 +896,19 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -1449,7 +1529,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6B45-41BC-832C-225F9A2781F9}"/>
             </c:ext>
@@ -1463,17 +1543,41 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="451451312"/>
-        <c:axId val="451450920"/>
+        <c:axId val="278523064"/>
+        <c:axId val="278522280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451451312"/>
+        <c:axId val="278523064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1500,6 +1604,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1566,7 +1671,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451450920"/>
+        <c:crossAx val="278522280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1574,7 +1679,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="451450920"/>
+        <c:axId val="278522280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1620,6 +1725,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1650,7 +1756,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1680,7 +1786,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451451312"/>
+        <c:crossAx val="278523064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1694,6 +1800,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1761,7 +1868,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1774,6 +1881,67 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Simulation</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 3</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1885,7 +2053,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-960B-41ED-823D-839B865DE580}"/>
             </c:ext>
@@ -1996,7 +2164,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-960B-41ED-823D-839B865DE580}"/>
             </c:ext>
@@ -2012,16 +2180,30 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="451450528"/>
-        <c:axId val="455091536"/>
+        <c:axId val="278526984"/>
+        <c:axId val="278523456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="451450528"/>
+        <c:axId val="278526984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2048,6 +2230,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2114,7 +2297,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455091536"/>
+        <c:crossAx val="278523456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2122,7 +2305,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455091536"/>
+        <c:axId val="278523456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2168,6 +2351,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2228,7 +2412,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="451450528"/>
+        <c:crossAx val="278526984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2242,6 +2426,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2309,7 +2494,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2322,6 +2507,62 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Simulation 2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2439,7 +2680,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-02CA-400C-8370-65A4633155B9}"/>
             </c:ext>
@@ -2556,7 +2797,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-02CA-400C-8370-65A4633155B9}"/>
             </c:ext>
@@ -2572,16 +2813,30 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="455091144"/>
-        <c:axId val="455092320"/>
+        <c:axId val="278525024"/>
+        <c:axId val="278524240"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="455091144"/>
+        <c:axId val="278525024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2608,6 +2863,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2674,7 +2930,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455092320"/>
+        <c:crossAx val="278524240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2682,7 +2938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="455092320"/>
+        <c:axId val="278524240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2728,6 +2984,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2788,7 +3045,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="455091144"/>
+        <c:crossAx val="278525024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2802,6 +3059,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2869,7 +3127,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2882,6 +3140,62 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Simulation 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -2926,6 +3240,75 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$178:$A$197</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$L$178:$L$197</c:f>
@@ -2996,7 +3379,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-BEAC-4744-AD0D-DE399E84869D}"/>
             </c:ext>
@@ -3040,6 +3423,75 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$178:$A$197</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Sheet1!$M$178:$M$197</c:f>
@@ -3110,7 +3562,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-BEAC-4744-AD0D-DE399E84869D}"/>
             </c:ext>
@@ -3126,16 +3578,30 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="742790920"/>
-        <c:axId val="742792712"/>
+        <c:axId val="278523848"/>
+        <c:axId val="278521888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="742790920"/>
+        <c:axId val="278523848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -3162,6 +3628,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3191,6 +3658,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3227,7 +3695,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="742792712"/>
+        <c:crossAx val="278521888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3235,7 +3703,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="742792712"/>
+        <c:axId val="278521888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3281,6 +3749,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3341,7 +3810,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="742790920"/>
+        <c:crossAx val="278523848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3355,6 +3824,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3582,7 +4052,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -3690,11 +4160,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -3705,11 +4170,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -3741,9 +4201,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5617,16 +6074,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>117</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="10" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAEBE615-CCF8-42FA-A944-2292BF4492F3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FAEBE615-CCF8-42FA-A944-2292BF4492F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5653,16 +6110,16 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>173</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>95251</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9805B242-F566-4ADC-A690-9F74C4128B1B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9805B242-F566-4ADC-A690-9F74C4128B1B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5683,22 +6140,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>542924</xdr:colOff>
       <xdr:row>130</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A347DF2D-1F64-4B04-8204-7195C4C26A31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A347DF2D-1F64-4B04-8204-7195C4C26A31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5719,14 +6176,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>942975</xdr:colOff>
+      <xdr:colOff>942974</xdr:colOff>
       <xdr:row>198</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>213</xdr:row>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>215</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -5734,7 +6191,7 @@
         <xdr:cNvPr id="3" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05908722-FFD6-41B7-A1A9-E865F592B14C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{05908722-FFD6-41B7-A1A9-E865F592B14C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5831,23 +6288,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5883,23 +6323,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6054,11 +6477,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
-      <selection activeCell="L177" sqref="L177:M197"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H174" sqref="H174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
@@ -6070,12 +6493,12 @@
     <col min="14" max="14" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -6110,7 +6533,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -6149,7 +6572,7 @@
         <v>4.206666666666667</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -6188,7 +6611,7 @@
         <v>6.4133333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15</v>
       </c>
@@ -6227,7 +6650,7 @@
         <v>8.3733333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>20</v>
       </c>
@@ -6266,7 +6689,7 @@
         <v>11.183333333333332</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -6305,7 +6728,7 @@
         <v>13.520000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -6344,7 +6767,7 @@
         <v>16.626666666666665</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -6383,7 +6806,7 @@
         <v>18.349999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -6422,7 +6845,7 @@
         <v>20.966666666666669</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>45</v>
       </c>
@@ -6461,7 +6884,7 @@
         <v>24.303333333333331</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
@@ -6500,7 +6923,7 @@
         <v>26.41</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>55</v>
       </c>
@@ -6539,7 +6962,7 @@
         <v>29.393333333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>60</v>
       </c>
@@ -6578,7 +7001,7 @@
         <v>31.349999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>65</v>
       </c>
@@ -6617,7 +7040,7 @@
         <v>33.96</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>70</v>
       </c>
@@ -6656,7 +7079,7 @@
         <v>35.633333333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>75</v>
       </c>
@@ -6695,7 +7118,7 @@
         <v>38.743333333333332</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>80</v>
       </c>
@@ -6734,7 +7157,7 @@
         <v>41.19</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>85</v>
       </c>
@@ -6773,7 +7196,7 @@
         <v>44.406666666666666</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>90</v>
       </c>
@@ -6812,7 +7235,7 @@
         <v>46.936666666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>95</v>
       </c>
@@ -6851,7 +7274,7 @@
         <v>49.246666666666663</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>100</v>
       </c>
@@ -6890,7 +7313,7 @@
         <v>51.636666666666663</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>105</v>
       </c>
@@ -6929,7 +7352,7 @@
         <v>54.196666666666665</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>110</v>
       </c>
@@ -6968,7 +7391,7 @@
         <v>56.476666666666667</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>115</v>
       </c>
@@ -7007,7 +7430,7 @@
         <v>58.32</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>120</v>
       </c>
@@ -7046,7 +7469,7 @@
         <v>61.533333333333339</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>125</v>
       </c>
@@ -7085,7 +7508,7 @@
         <v>63.389999999999993</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>130</v>
       </c>
@@ -7124,7 +7547,7 @@
         <v>66.509999999999991</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>135</v>
       </c>
@@ -7163,7 +7586,7 @@
         <v>68.873333333333335</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>140</v>
       </c>
@@ -7202,7 +7625,7 @@
         <v>71.023333333333326</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>145</v>
       </c>
@@ -7241,7 +7664,7 @@
         <v>73.600000000000009</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>150</v>
       </c>
@@ -7280,7 +7703,7 @@
         <v>75.916666666666671</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>155</v>
       </c>
@@ -7319,7 +7742,7 @@
         <v>77.83</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>160</v>
       </c>
@@ -7358,7 +7781,7 @@
         <v>80.186666666666667</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>165</v>
       </c>
@@ -7397,7 +7820,7 @@
         <v>82.576666666666668</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>170</v>
       </c>
@@ -7436,7 +7859,7 @@
         <v>84.823333333333338</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>175</v>
       </c>
@@ -7475,7 +7898,7 @@
         <v>86.776666666666657</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>180</v>
       </c>
@@ -7514,7 +7937,7 @@
         <v>89.826666666666668</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>185</v>
       </c>
@@ -7553,7 +7976,7 @@
         <v>92.473333333333343</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>190</v>
       </c>
@@ -7592,7 +8015,7 @@
         <v>95.333333333333329</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>195</v>
       </c>
@@ -7631,7 +8054,7 @@
         <v>97.906666666666652</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>200</v>
       </c>
@@ -7670,7 +8093,7 @@
         <v>99.793333333333337</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>205</v>
       </c>
@@ -7709,7 +8132,7 @@
         <v>101.80000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>210</v>
       </c>
@@ -7748,7 +8171,7 @@
         <v>103.86333333333334</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>215</v>
       </c>
@@ -7787,7 +8210,7 @@
         <v>107.04333333333334</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>220</v>
       </c>
@@ -7826,7 +8249,7 @@
         <v>109.35666666666667</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>225</v>
       </c>
@@ -7865,7 +8288,7 @@
         <v>111.96</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>230</v>
       </c>
@@ -7904,7 +8327,7 @@
         <v>114.33666666666666</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>235</v>
       </c>
@@ -7943,7 +8366,7 @@
         <v>116.65000000000002</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>240</v>
       </c>
@@ -7982,7 +8405,7 @@
         <v>119.44666666666666</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>245</v>
       </c>
@@ -8021,7 +8444,7 @@
         <v>122.12666666666667</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>250</v>
       </c>
@@ -8060,7 +8483,7 @@
         <v>124.53333333333335</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>255</v>
       </c>
@@ -8099,7 +8522,7 @@
         <v>128.04</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>260</v>
       </c>
@@ -8138,7 +8561,7 @@
         <v>130.40666666666667</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>265</v>
       </c>
@@ -8177,7 +8600,7 @@
         <v>133.47999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>270</v>
       </c>
@@ -8216,7 +8639,7 @@
         <v>135.14666666666668</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>275</v>
       </c>
@@ -8255,7 +8678,7 @@
         <v>138.12</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>280</v>
       </c>
@@ -8294,7 +8717,7 @@
         <v>140.13</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>285</v>
       </c>
@@ -8333,7 +8756,7 @@
         <v>143.33333333333334</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>290</v>
       </c>
@@ -8372,7 +8795,7 @@
         <v>145.76</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>295</v>
       </c>
@@ -8411,7 +8834,7 @@
         <v>147.91999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>300</v>
       </c>
@@ -8450,7 +8873,7 @@
         <v>150.23666666666665</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>305</v>
       </c>
@@ -8489,7 +8912,7 @@
         <v>153.28</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>310</v>
       </c>
@@ -8528,7 +8951,7 @@
         <v>155.96</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>315</v>
       </c>
@@ -8567,7 +8990,7 @@
         <v>158.53666666666666</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>320</v>
       </c>
@@ -8606,7 +9029,7 @@
         <v>160.76</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>325</v>
       </c>
@@ -8645,7 +9068,7 @@
         <v>162.37666666666669</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>330</v>
       </c>
@@ -8684,7 +9107,7 @@
         <v>164.91</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>335</v>
       </c>
@@ -8723,7 +9146,7 @@
         <v>167.89000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>340</v>
       </c>
@@ -8762,7 +9185,7 @@
         <v>170.22333333333333</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>345</v>
       </c>
@@ -8801,7 +9224,7 @@
         <v>173.16</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>350</v>
       </c>
@@ -8840,7 +9263,7 @@
         <v>175.43333333333331</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>355</v>
       </c>
@@ -8879,7 +9302,7 @@
         <v>178.05333333333331</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>360</v>
       </c>
@@ -8918,7 +9341,7 @@
         <v>180.35666666666665</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>365</v>
       </c>
@@ -8957,7 +9380,7 @@
         <v>182.45000000000002</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>370</v>
       </c>
@@ -8996,7 +9419,7 @@
         <v>184.53333333333333</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>375</v>
       </c>
@@ -9035,7 +9458,7 @@
         <v>187.50666666666666</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>380</v>
       </c>
@@ -9074,7 +9497,7 @@
         <v>189.70666666666668</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>385</v>
       </c>
@@ -9113,7 +9536,7 @@
         <v>193.24</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>390</v>
       </c>
@@ -9152,7 +9575,7 @@
         <v>195.55333333333337</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>395</v>
       </c>
@@ -9191,7 +9614,7 @@
         <v>198.62666666666667</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>400</v>
       </c>
@@ -9230,7 +9653,7 @@
         <v>200.43333333333331</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>405</v>
       </c>
@@ -9269,7 +9692,7 @@
         <v>203.53333333333333</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>410</v>
       </c>
@@ -9308,7 +9731,7 @@
         <v>205.82000000000002</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>415</v>
       </c>
@@ -9347,7 +9770,7 @@
         <v>207.70666666666668</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>420</v>
       </c>
@@ -9386,7 +9809,7 @@
         <v>210.26333333333332</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>425</v>
       </c>
@@ -9425,7 +9848,7 @@
         <v>212.71333333333337</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>430</v>
       </c>
@@ -9464,7 +9887,7 @@
         <v>215.14666666666668</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>435</v>
       </c>
@@ -9503,7 +9926,7 @@
         <v>217.94000000000003</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>440</v>
       </c>
@@ -9542,7 +9965,7 @@
         <v>220.86333333333334</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>445</v>
       </c>
@@ -9581,7 +10004,7 @@
         <v>222.57666666666668</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>450</v>
       </c>
@@ -9620,7 +10043,7 @@
         <v>225.02</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>455</v>
       </c>
@@ -9659,7 +10082,7 @@
         <v>227.19666666666669</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>460</v>
       </c>
@@ -9698,7 +10121,7 @@
         <v>229.84</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>465</v>
       </c>
@@ -9737,7 +10160,7 @@
         <v>232.42333333333332</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>470</v>
       </c>
@@ -9776,7 +10199,7 @@
         <v>234.60666666666665</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>475</v>
       </c>
@@ -9815,7 +10238,7 @@
         <v>237.52666666666664</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>480</v>
       </c>
@@ -9854,7 +10277,7 @@
         <v>240.03</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>485</v>
       </c>
@@ -9893,7 +10316,7 @@
         <v>242.67999999999998</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>490</v>
       </c>
@@ -9932,7 +10355,7 @@
         <v>244.90333333333334</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>495</v>
       </c>
@@ -9971,7 +10394,7 @@
         <v>247.91333333333333</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>500</v>
       </c>
@@ -10010,12 +10433,12 @@
         <v>250.76666666666665</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -10050,7 +10473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2</v>
       </c>
@@ -10089,7 +10512,7 @@
         <v>109.63333333333333</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>3</v>
       </c>
@@ -10128,7 +10551,7 @@
         <v>58.589999999999996</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>4</v>
       </c>
@@ -10167,7 +10590,7 @@
         <v>51.713333333333331</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>5</v>
       </c>
@@ -10206,7 +10629,7 @@
         <v>50.370000000000005</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>6</v>
       </c>
@@ -10245,7 +10668,7 @@
         <v>50.56</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>7</v>
       </c>
@@ -10284,7 +10707,7 @@
         <v>50.379999999999995</v>
       </c>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>8</v>
       </c>
@@ -10323,7 +10746,7 @@
         <v>50.613333333333337</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>9</v>
       </c>
@@ -10362,7 +10785,7 @@
         <v>50.713333333333331</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>10</v>
       </c>
@@ -10401,12 +10824,12 @@
         <v>51.436666666666667</v>
       </c>
     </row>
-    <row r="148" spans="1:14">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="149" spans="1:14">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>14</v>
       </c>
@@ -10414,7 +10837,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="30">
+    <row r="150" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>1</v>
       </c>
@@ -10446,7 +10869,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="151" spans="1:14">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>5</v>
       </c>
@@ -10488,7 +10911,7 @@
         <v>2.1333333333333333</v>
       </c>
     </row>
-    <row r="152" spans="1:14">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>10</v>
       </c>
@@ -10530,7 +10953,7 @@
         <v>3.3333333333333335</v>
       </c>
     </row>
-    <row r="153" spans="1:14">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>15</v>
       </c>
@@ -10572,7 +10995,7 @@
         <v>4.1333333333333337</v>
       </c>
     </row>
-    <row r="154" spans="1:14">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>20</v>
       </c>
@@ -10614,7 +11037,7 @@
         <v>5.5999999999999988</v>
       </c>
     </row>
-    <row r="155" spans="1:14">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>25</v>
       </c>
@@ -10656,7 +11079,7 @@
         <v>6.7333333333333343</v>
       </c>
     </row>
-    <row r="156" spans="1:14">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>30</v>
       </c>
@@ -10698,7 +11121,7 @@
         <v>7.3999999999999995</v>
       </c>
     </row>
-    <row r="157" spans="1:14">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>35</v>
       </c>
@@ -10740,7 +11163,7 @@
         <v>8.6</v>
       </c>
     </row>
-    <row r="158" spans="1:14">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>40</v>
       </c>
@@ -10782,12 +11205,12 @@
         <v>36.133333333333333</v>
       </c>
     </row>
-    <row r="176" spans="1:1">
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>1</v>
       </c>
@@ -10822,7 +11245,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>5</v>
       </c>
@@ -10861,7 +11284,7 @@
         <v>4.7733333333333334</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>10</v>
       </c>
@@ -10900,7 +11323,7 @@
         <v>7.4699999999999989</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>15</v>
       </c>
@@ -10939,7 +11362,7 @@
         <v>10.213333333333333</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>20</v>
       </c>
@@ -10978,7 +11401,7 @@
         <v>14.780000000000001</v>
       </c>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>25</v>
       </c>
@@ -11017,7 +11440,7 @@
         <v>17.040000000000003</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>30</v>
       </c>
@@ -11056,7 +11479,7 @@
         <v>21.403333333333336</v>
       </c>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>35</v>
       </c>
@@ -11095,7 +11518,7 @@
         <v>24.583333333333332</v>
       </c>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>40</v>
       </c>
@@ -11134,7 +11557,7 @@
         <v>27.286666666666665</v>
       </c>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>45</v>
       </c>
@@ -11173,7 +11596,7 @@
         <v>29.973333333333333</v>
       </c>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>50</v>
       </c>
@@ -11212,7 +11635,7 @@
         <v>33.92</v>
       </c>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>55</v>
       </c>
@@ -11251,7 +11674,7 @@
         <v>37.21</v>
       </c>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>30</v>
       </c>
@@ -11290,7 +11713,7 @@
         <v>39.956666666666671</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>65</v>
       </c>
@@ -11329,7 +11752,7 @@
         <v>43.419999999999995</v>
       </c>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>70</v>
       </c>
@@ -11368,7 +11791,7 @@
         <v>45.586666666666666</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>75</v>
       </c>
@@ -11407,7 +11830,7 @@
         <v>48.49666666666667</v>
       </c>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>80</v>
       </c>
@@ -11446,7 +11869,7 @@
         <v>51.803333333333335</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>85</v>
       </c>
@@ -11485,7 +11908,7 @@
         <v>54.04</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>90</v>
       </c>
@@ -11524,7 +11947,7 @@
         <v>56.856666666666662</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>95</v>
       </c>
@@ -11563,7 +11986,7 @@
         <v>59.073333333333331</v>
       </c>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>100</v>
       </c>
@@ -11618,12 +12041,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A93D09C51E9DB340B91D5179D32101FD" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0e7cb0e9035549e77d64d4d70348c1d5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="499237529fc265eb263c4c2e11b70e13">
     <xsd:element name="properties">
@@ -11737,6 +12154,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{61B8C2E4-C400-4ABF-801B-0D407BA97C0D}">
   <ds:schemaRefs>
@@ -11746,15 +12169,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F712D97A-EE25-4176-8AD3-8D0B3F81E247}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DDE555B-2896-43D2-B00F-7D45187B9043}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11768,4 +12182,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F712D97A-EE25-4176-8AD3-8D0B3F81E247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>